<commit_message>
added a user story
</commit_message>
<xml_diff>
--- a/08_MiscDocs/user_stories_long_term_effort_estimation.xlsx
+++ b/08_MiscDocs/user_stories_long_term_effort_estimation.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25028"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25128"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Dominik\Documents\Schule\SYP\if.05.61_01-project-repository\08_MiscDocs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{768D818A-B83D-47E1-AEFC-56A49C6CB172}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{864B1A28-6AAC-43AE-883C-685CD8621D6B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{5FD58B51-89EC-47EC-B4DB-862D99256616}"/>
   </bookViews>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="17" uniqueCount="14">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="17">
   <si>
     <t>ID</t>
   </si>
@@ -77,6 +77,15 @@
   </si>
   <si>
     <t>Simulation can run in realtime(performance!) changeable spead</t>
+  </si>
+  <si>
+    <t>modeller</t>
+  </si>
+  <si>
+    <t>As a modeller I want to compare my output to a reliable simulation, where I used similar parameters.</t>
+  </si>
+  <si>
+    <t>cloned other simulation from github, changed parameters and compared results</t>
   </si>
 </sst>
 </file>
@@ -112,7 +121,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -122,6 +131,9 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -535,10 +547,21 @@
         <v>1</v>
       </c>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="E6">
-        <f>SUM(E2:E5)</f>
-        <v>10</v>
+    <row r="6" spans="1:5" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A6" s="2">
+        <v>7</v>
+      </c>
+      <c r="B6" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="C6" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="D6" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="E6" s="4">
+        <v>8</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Made Events visible on UI and added TestPerson to track movements of a person
</commit_message>
<xml_diff>
--- a/08_MiscDocs/user_stories_long_term_effort_estimation.xlsx
+++ b/08_MiscDocs/user_stories_long_term_effort_estimation.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Dominik\Documents\Schule\SYP\if.05.61_01-project-repository\08_MiscDocs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{864B1A28-6AAC-43AE-883C-685CD8621D6B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0BC86312-4DD6-4734-BD1C-E4D35672913C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{5FD58B51-89EC-47EC-B4DB-862D99256616}"/>
   </bookViews>
@@ -452,14 +452,16 @@
   <dimension ref="A1:E6"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="E6" sqref="E6"/>
+      <selection activeCell="F4" sqref="F4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
+    <col min="1" max="1" width="4.77734375" customWidth="1"/>
+    <col min="2" max="2" width="9" customWidth="1"/>
     <col min="3" max="3" width="70" style="1" customWidth="1"/>
     <col min="4" max="4" width="49" style="1" customWidth="1"/>
-    <col min="5" max="5" width="49" customWidth="1"/>
+    <col min="5" max="5" width="9.77734375" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.3">

</xml_diff>